<commit_message>
update doc, fix delete view
</commit_message>
<xml_diff>
--- a/doc/book解析.xlsx
+++ b/doc/book解析.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\user1\work\workspace\git\bookproject\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E361883-2D1C-46EE-8DD9-829A84AA9479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E1D1D7-B52A-4ED0-BB8B-86C7C2DD13F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="548" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="548" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="views.py" sheetId="8" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="284">
   <si>
     <r>
       <t>from</t>
@@ -2818,137 +2818,6 @@
         <family val="3"/>
       </rPr>
       <t>"create-book"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>),</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDCDCAA"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>path</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCE9178"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>"book/&lt;int:pk&gt;/delete/"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4EC9B0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>views</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4EC9B0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>DetailBookView</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDCDCAA"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>as_view</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">(), </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF9CDCFE"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>name</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD4D4D4"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCE9178"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>"delete-book"</t>
     </r>
     <r>
       <rPr>
@@ -9081,6 +8950,176 @@
     <rPh sb="18" eb="19">
       <t>ヒモ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>urlとビューの紐づけ用</t>
+    <rPh sb="8" eb="9">
+      <t>ヒモ</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>ヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>viewのクラスをimport</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>トップページ（ルートURL）へのアクセスを index_view で処理。
+name="index" によって、テンプレートなどで url 'index' として逆引き可能。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>↑以下同様</t>
+    <rPh sb="1" eb="3">
+      <t>イカ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ドウヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">↑ + 特定の書籍の詳細ページ。&lt;int:pk&gt; で主キー（Primary Key）をURLから取得。
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>↑+ 特定の書籍の詳細ページ。&lt;int:pk&gt; で主キー（Primary Key）をURLから取得。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFDCDCAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>path</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"book/&lt;int:pk&gt;/delete/"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4EC9B0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>views</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4EC9B0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>DeleteBookView</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFDCDCAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>as_view</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">(), </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"delete-book"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>),</t>
+    </r>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -15720,168 +15759,168 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="B2" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="B3" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="B4" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="B5" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="37.5">
       <c r="B6" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="37.5">
       <c r="B7" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="B8" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="B9" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="B10" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="B11" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="B12" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="B13" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="B14" s="2"/>
       <c r="C14" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="B15" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -15889,1536 +15928,1536 @@
         <v>1</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="2:21">
       <c r="B17" s="2"/>
       <c r="C17" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="2:21">
       <c r="B18" s="2"/>
       <c r="C18" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="2:21">
       <c r="B19" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20" spans="2:21">
       <c r="B20" s="2"/>
       <c r="C20" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="2:21">
       <c r="B21" s="2"/>
       <c r="C21" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="2:21">
       <c r="B22" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="23" spans="2:21" ht="75">
       <c r="B23" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="2:21">
       <c r="B24" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="2:21">
       <c r="B25" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="2:21">
       <c r="B26" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="27" spans="2:21">
       <c r="B27" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="28" spans="2:21">
       <c r="B28" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D28" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="29" spans="2:21" ht="378.75">
       <c r="B29" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C29" s="13" t="s">
         <v>145</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="30" spans="2:21">
       <c r="B30" s="2"/>
       <c r="C30" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D30" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="T30" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="U30" s="18" t="s">
         <v>157</v>
-      </c>
-      <c r="U30" s="18" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="31" spans="2:21" ht="37.5">
       <c r="B31" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="T31" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="U31" s="19" t="s">
         <v>159</v>
-      </c>
-      <c r="U31" s="19" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="32" spans="2:21" ht="37.5">
       <c r="B32" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="T32" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="U32" s="19" t="s">
         <v>161</v>
-      </c>
-      <c r="U32" s="19" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="33" spans="2:21" ht="37.5">
       <c r="B33" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="T33" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="U33" s="19" t="s">
         <v>163</v>
-      </c>
-      <c r="U33" s="19" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="34" spans="2:21">
       <c r="B34" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D34" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="35" spans="2:21">
       <c r="B35" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D35" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="2:21">
       <c r="B36" s="2"/>
       <c r="C36" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D36" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="37" spans="2:21">
       <c r="B37" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D37" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="38" spans="2:21" ht="165.75">
       <c r="B38" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="39" spans="2:21" ht="112.5">
       <c r="B39" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="C39" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="C39" s="12" t="s">
-        <v>155</v>
-      </c>
       <c r="D39" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="40" spans="2:21" ht="75">
       <c r="B40" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D40" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="41" spans="2:21">
       <c r="B41" s="2"/>
       <c r="C41" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D41" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="42" spans="2:21">
       <c r="B42" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D42" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="43" spans="2:21" ht="56.25">
       <c r="B43" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D43" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="44" spans="2:21">
       <c r="B44" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="45" spans="2:21">
       <c r="B45" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D45" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="46" spans="2:21" ht="75">
       <c r="B46" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C46" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="C46" s="12" t="s">
-        <v>148</v>
-      </c>
       <c r="D46" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="47" spans="2:21">
       <c r="B47" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D47" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="48" spans="2:21">
       <c r="B48" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D48" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="49" spans="2:4">
       <c r="B49" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D49" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="50" spans="2:4">
       <c r="B50" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D50" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="51" spans="2:4" ht="141.75" customHeight="1">
       <c r="B51" s="2"/>
       <c r="C51" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D51" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="52" spans="2:4" ht="141.75" customHeight="1">
       <c r="B52" s="2"/>
       <c r="C52" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D52" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="53" spans="2:4">
       <c r="B53" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D53" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="54" spans="2:4">
       <c r="B54" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D54" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="55" spans="2:4" ht="56.25">
       <c r="B55" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D55" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="56" spans="2:4" ht="168.75">
       <c r="B56" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D56" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="57" spans="2:4" ht="112.5">
       <c r="B57" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D57" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="58" spans="2:4">
       <c r="B58" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D58" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="59" spans="2:4">
       <c r="B59" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D59" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="60" spans="2:4">
       <c r="B60" s="2"/>
       <c r="C60" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D60" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="61" spans="2:4">
       <c r="B61" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D61" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="62" spans="2:4" ht="243.75">
       <c r="B62" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="C62" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="C62" s="11" t="s">
-        <v>175</v>
-      </c>
       <c r="D62" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="63" spans="2:4" ht="131.25">
       <c r="B63" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D63" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="64" spans="2:4">
       <c r="B64" s="2"/>
       <c r="C64" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D64" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="65" spans="2:21">
       <c r="B65" s="2"/>
       <c r="C65" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D65" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="66" spans="2:21">
       <c r="B66" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D66" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="67" spans="2:21" ht="150">
       <c r="B67" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D67" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="T67" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="U67" s="14" t="s">
         <v>177</v>
-      </c>
-      <c r="U67" s="14" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="68" spans="2:21" ht="37.5">
       <c r="B68" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D68" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="T68" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="U68" s="15" t="s">
         <v>179</v>
-      </c>
-      <c r="U68" s="15" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="69" spans="2:21" ht="75">
       <c r="B69" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D69" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="T69" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="U69" s="15" t="s">
         <v>181</v>
-      </c>
-      <c r="U69" s="15" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="70" spans="2:21" ht="56.25">
       <c r="B70" s="2"/>
       <c r="C70" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D70" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="T70" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="U70" s="15" t="s">
         <v>183</v>
-      </c>
-      <c r="U70" s="15" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="71" spans="2:21" ht="37.5">
       <c r="B71" s="2"/>
       <c r="C71" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D71" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="T71" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="U71" s="15" t="s">
         <v>185</v>
-      </c>
-      <c r="U71" s="15" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="72" spans="2:21" ht="37.5">
       <c r="B72" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D72" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="T72" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="U72" s="15" t="s">
         <v>187</v>
-      </c>
-      <c r="U72" s="15" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="73" spans="2:21" ht="187.5">
       <c r="B73" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D73" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E73" s="11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="74" spans="2:21">
       <c r="B74" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D74" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="75" spans="2:21">
       <c r="B75" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D75" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="76" spans="2:21" ht="75">
       <c r="B76" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="C76" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="C76" s="12" t="s">
-        <v>199</v>
-      </c>
       <c r="D76" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="77" spans="2:21">
       <c r="B77" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D77" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="78" spans="2:21">
       <c r="B78" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C78" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D78" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="79" spans="2:21">
       <c r="B79" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D79" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="80" spans="2:21">
       <c r="B80" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C80" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D80" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="81" spans="2:5" ht="187.5">
       <c r="B81" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C81" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D81" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="82" spans="2:5">
       <c r="B82" s="2"/>
       <c r="C82" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D82" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="83" spans="2:5">
       <c r="B83" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D83" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="84" spans="2:5">
       <c r="B84" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C84" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D84" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="85" spans="2:5" ht="177" customHeight="1">
       <c r="B85" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D85" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E85" s="11"/>
     </row>
     <row r="86" spans="2:5" ht="56.25">
       <c r="B86" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="C86" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="C86" s="12" t="s">
-        <v>202</v>
-      </c>
       <c r="D86" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="87" spans="2:5" ht="37.5">
       <c r="B87" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C87" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D87" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="88" spans="2:5">
       <c r="B88" s="2"/>
       <c r="C88" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D88" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="89" spans="2:5">
       <c r="B89" s="2"/>
       <c r="C89" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D89" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="90" spans="2:5">
       <c r="B90" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C90" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D90" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="91" spans="2:5" ht="112.5">
       <c r="B91" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C91" s="11" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D91" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="92" spans="2:5" ht="75">
       <c r="B92" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C92" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D92" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="93" spans="2:5" ht="56.25">
       <c r="B93" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C93" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D93" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="94" spans="2:5" ht="131.25">
       <c r="B94" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D94" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="95" spans="2:5">
       <c r="B95" s="2"/>
       <c r="C95" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D95" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="96" spans="2:5">
       <c r="B96" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C96" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D96" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="97" spans="2:4" ht="131.25">
       <c r="B97" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C97" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="C97" s="11" t="s">
-        <v>213</v>
-      </c>
       <c r="D97" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="98" spans="2:4" ht="37.5">
       <c r="B98" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C98" s="11" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D98" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="99" spans="2:4">
       <c r="B99" s="2"/>
       <c r="C99" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D99" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="100" spans="2:4" ht="93.75">
       <c r="B100" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C100" s="11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D100" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="101" spans="2:4">
       <c r="B101" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C101" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D101" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="102" spans="2:4">
       <c r="B102" s="2"/>
       <c r="C102" s="11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D102" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="103" spans="2:4">
       <c r="B103" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C103" s="11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D103" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="104" spans="2:4">
       <c r="B104" s="2"/>
       <c r="C104" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D104" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="105" spans="2:4">
       <c r="B105" s="2"/>
       <c r="C105" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D105" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="106" spans="2:4">
       <c r="B106" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C106" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D106" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="107" spans="2:4" ht="150">
       <c r="B107" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C107" s="11" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D107" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="108" spans="2:4">
       <c r="B108" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C108" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D108" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="109" spans="2:4">
       <c r="B109" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C109" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="C109" s="11" t="s">
-        <v>218</v>
-      </c>
       <c r="D109" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="110" spans="2:4">
       <c r="B110" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C110" s="11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D110" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="111" spans="2:4">
       <c r="B111" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C111" s="11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D111" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="112" spans="2:4">
       <c r="B112" s="2"/>
       <c r="C112" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D112" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="113" spans="2:22">
       <c r="B113" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C113" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D113" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="114" spans="2:22" ht="37.5">
       <c r="B114" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C114" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D114" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="115" spans="2:22">
       <c r="B115" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C115" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D115" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="116" spans="2:22">
       <c r="B116" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C116" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D116" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="117" spans="2:22">
       <c r="B117" s="2"/>
       <c r="C117" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D117" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="118" spans="2:22">
       <c r="B118" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C118" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D118" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="119" spans="2:22">
       <c r="B119" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C119" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D119" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="120" spans="2:22">
       <c r="B120" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C120" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D120" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="121" spans="2:22">
       <c r="B121" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C121" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D121" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="122" spans="2:22">
       <c r="B122" s="2"/>
       <c r="C122" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D122" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="T122" s="14"/>
       <c r="U122" s="14"/>
       <c r="V122" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="123" spans="2:22" ht="56.25">
       <c r="B123" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C123" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D123" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="T123" s="15"/>
       <c r="U123" s="15"/>
       <c r="V123" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="124" spans="2:22" ht="56.25">
       <c r="B124" s="2"/>
       <c r="C124" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D124" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="T124" s="15"/>
       <c r="U124" s="15"/>
       <c r="V124" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="125" spans="2:22">
       <c r="B125" s="2"/>
       <c r="C125" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D125" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="126" spans="2:22">
       <c r="B126" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C126" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D126" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="127" spans="2:22" ht="93.75">
       <c r="B127" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C127" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D127" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="128" spans="2:22" ht="37.5">
       <c r="B128" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C128" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D128" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="129" spans="2:4">
       <c r="B129" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C129" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D129" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="130" spans="2:4">
       <c r="B130" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C130" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D130" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="131" spans="2:4">
       <c r="B131" s="2"/>
       <c r="C131" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D131" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="132" spans="2:4">
       <c r="B132" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C132" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D132" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="133" spans="2:4">
       <c r="B133" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C133" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D133" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="134" spans="2:4">
       <c r="B134" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C134" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="D134" t="s">
         <v>250</v>
-      </c>
-      <c r="D134" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="135" spans="2:4">
       <c r="B135" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D135" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="136" spans="2:4">
       <c r="B136" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C136" s="12" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D136" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="137" spans="2:4">
       <c r="B137" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C137" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D137" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="138" spans="2:4" ht="93.75">
       <c r="B138" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C138" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D138" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="139" spans="2:4">
       <c r="B139" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C139" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D139" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="140" spans="2:4">
       <c r="B140" s="2"/>
       <c r="C140" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D140" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="141" spans="2:4">
       <c r="B141" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C141" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D141" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="142" spans="2:4">
       <c r="B142" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C142" s="11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D142" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="143" spans="2:4">
       <c r="B143" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C143" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D143" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="144" spans="2:4">
       <c r="B144" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C144" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D144" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="145" spans="2:4" ht="56.25">
       <c r="B145" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C145" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D145" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="146" spans="2:4">
       <c r="B146" s="2"/>
       <c r="C146" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D146" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="147" spans="2:4" ht="37.5">
       <c r="B147" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C147" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D147" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="148" spans="2:4">
       <c r="B148" s="2"/>
       <c r="C148" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D148" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="149" spans="2:4">
       <c r="B149" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C149" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D149" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="150" spans="2:4" ht="37.5">
       <c r="B150" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C150" s="11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D150" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="151" spans="2:4" ht="56.25">
       <c r="B151" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C151" s="11" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D151" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="186" spans="5:7">
       <c r="E186" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="F186" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="G186" s="14" t="s">
         <v>233</v>
-      </c>
-      <c r="F186" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="G186" s="14" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="187" spans="5:7" ht="75">
       <c r="E187" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="F187" s="15" t="s">
         <v>235</v>
       </c>
-      <c r="F187" s="15" t="s">
+      <c r="G187" s="16" t="s">
         <v>236</v>
-      </c>
-      <c r="G187" s="16" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="188" spans="5:7" ht="75">
       <c r="E188" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="F188" s="15" t="s">
         <v>238</v>
       </c>
-      <c r="F188" s="15" t="s">
+      <c r="G188" s="15" t="s">
         <v>239</v>
-      </c>
-      <c r="G188" s="15" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="190" spans="5:7" ht="30">
@@ -17426,34 +17465,34 @@
     </row>
     <row r="192" spans="5:7">
       <c r="E192" s="14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F192" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="193" spans="5:6" ht="93.75">
       <c r="E193" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="F193" s="15" t="s">
         <v>243</v>
-      </c>
-      <c r="F193" s="15" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="194" spans="5:6" ht="44.25">
       <c r="E194" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="F194" s="16" t="s">
         <v>245</v>
-      </c>
-      <c r="F194" s="16" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="195" spans="5:6" ht="93.75">
       <c r="E195" s="15" t="s">
+        <v>246</v>
+      </c>
+      <c r="F195" s="15" t="s">
         <v>247</v>
-      </c>
-      <c r="F195" s="15" t="s">
-        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -17477,16 +17516,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="37.5">
       <c r="A1" s="22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="37.5">
@@ -17494,19 +17533,19 @@
         <v>1</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="B3" s="2"/>
       <c r="C3" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="37.5">
@@ -17514,10 +17553,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -17525,10 +17564,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -17536,10 +17575,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -17562,34 +17601,34 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="B2" s="2"/>
       <c r="C2" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="B3" s="2"/>
       <c r="C3" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="37.5">
@@ -17597,10 +17636,10 @@
         <v>6</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="112.5">
@@ -17608,10 +17647,10 @@
         <v>7</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="37.5">
@@ -17619,10 +17658,10 @@
         <v>8</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -17646,16 +17685,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -17663,10 +17702,10 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -17674,19 +17713,19 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="B4" s="2"/>
       <c r="C4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -17694,10 +17733,10 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -17705,10 +17744,10 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -17721,7 +17760,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C3D3E1D-9BBA-44FA-954A-2211FC5D91F4}">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
@@ -17731,16 +17770,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -17748,28 +17787,28 @@
         <v>14</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="B3" s="2"/>
       <c r="C3" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="B4" s="2"/>
       <c r="C4" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -17777,10 +17816,10 @@
         <v>15</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -17788,10 +17827,10 @@
         <v>16</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -17799,19 +17838,19 @@
         <v>17</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="B8" s="2"/>
       <c r="C8" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -17819,10 +17858,10 @@
         <v>18</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="192.75" customHeight="1">
@@ -17830,28 +17869,28 @@
         <v>19</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="B11" s="2"/>
       <c r="C11" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="B12" s="2"/>
       <c r="C12" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -17859,21 +17898,21 @@
         <v>20</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="37.5">
       <c r="B14" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="37.5">
@@ -17881,10 +17920,10 @@
         <v>21</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="37.5">
@@ -17892,10 +17931,10 @@
         <v>33</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="56.25">
@@ -17903,10 +17942,10 @@
         <v>22</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="56.25">
@@ -17914,27 +17953,27 @@
         <v>23</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="C19" s="12" t="s">
         <v>276</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" s="2"/>
       <c r="C20" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="2:4">
@@ -17942,10 +17981,10 @@
         <v>24</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="37.5">
@@ -17953,10 +17992,10 @@
         <v>25</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="23" spans="2:4">
@@ -17964,28 +18003,28 @@
         <v>26</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" s="2"/>
       <c r="C24" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="2:4">
       <c r="B25" s="2"/>
       <c r="C25" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="2:4">
@@ -17993,10 +18032,10 @@
         <v>27</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="27" spans="2:4">
@@ -18004,10 +18043,10 @@
         <v>28</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="28" spans="2:4">
@@ -18015,10 +18054,10 @@
         <v>29</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D28" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="29" spans="2:4">
@@ -18026,10 +18065,10 @@
         <v>21</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D29" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" spans="2:4">
@@ -18037,10 +18076,10 @@
         <v>30</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D30" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="31" spans="2:4">
@@ -18048,10 +18087,10 @@
         <v>31</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="32" spans="2:4">
@@ -18059,16 +18098,16 @@
         <v>32</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="33" spans="2:4">
       <c r="B33" s="2"/>
       <c r="C33" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="37.5">
@@ -18076,10 +18115,10 @@
         <v>25</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D34" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="35" spans="2:4">
@@ -18087,10 +18126,10 @@
         <v>26</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D35" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -18102,96 +18141,201 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19D18F1E-50AC-4791-8792-7D25B1E84850}">
-  <dimension ref="B1:B17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
     <col min="2" max="2" width="107.875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="38.5" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2">
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>131</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="2:2">
+      <c r="C1" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="D1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="B2" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="2:2">
+      <c r="C2" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="D2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="2:2">
+      <c r="C3" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="D3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="B4" s="10" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="2:2">
+      <c r="D4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="75">
       <c r="B5" s="7" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6" spans="2:2">
+      <c r="C5" s="11" t="s">
+        <v>279</v>
+      </c>
+      <c r="D5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="B6" s="7" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="2:2">
+      <c r="C6" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="D6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="B7" s="7" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="8" spans="2:2">
+      <c r="C7" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="D7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="56.25">
       <c r="B8" s="7" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="2:2">
+      <c r="C8" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="D8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="B9" s="7" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="10" spans="2:2">
+      <c r="C9" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="D9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="37.5">
       <c r="B10" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>282</v>
+      </c>
+      <c r="D10" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="37.5">
+      <c r="B11" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="11" spans="2:2">
-      <c r="B11" s="7" t="s">
+      <c r="C11" s="11" t="s">
+        <v>282</v>
+      </c>
+      <c r="D11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="B12" s="7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="12" spans="2:2">
-      <c r="B12" s="7" t="s">
+      <c r="C12" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="D12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="B13" s="7" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="13" spans="2:2">
-      <c r="B13" s="7" t="s">
+      <c r="C13" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="D13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="B14" s="7" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="14" spans="2:2">
-      <c r="B14" s="7" t="s">
+      <c r="C14" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="D14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="B15" s="7" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="15" spans="2:2">
-      <c r="B15" s="7" t="s">
+      <c r="C15" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="D15" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="B16" s="7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="16" spans="2:2">
-      <c r="B16" s="7" t="s">
+      <c r="C16" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="D16" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="7" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="17" spans="2:2">
-      <c r="B17" s="7" t="s">
-        <v>49</v>
+      <c r="C17" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="D17" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>